<commit_message>
Updated software to make the relays, units, etc., from std::map to basic arrays. The individual devices are constants entries in the array. Updated the Schematic with vertical lines to separate the sections. Added the Williams Parts Catalog. Missing important pages in the Instruction Manual.  Need to make a copy of the one in the machine. Updated the Component Index with additional components.
</commit_message>
<xml_diff>
--- a/ComponentIndex.xlsx
+++ b/ComponentIndex.xlsx
@@ -8,15 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Craig\Documents\000 Pinball Troubleshooting\Sky_SpaceLab\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE261AFC-1C9F-48C4-9895-311504551643}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D22B9949-F59C-4084-B059-201A9B29C3A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1536" yWindow="1536" windowWidth="13044" windowHeight="12720" xr2:uid="{DF7D39D8-82A5-42A7-B8D6-78EEB1B66EE8}"/>
+    <workbookView xWindow="11700" yWindow="0" windowWidth="11436" windowHeight="13776" xr2:uid="{DF7D39D8-82A5-42A7-B8D6-78EEB1B66EE8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$5:$I$156</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="692" uniqueCount="234">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1003" uniqueCount="290">
   <si>
     <t>Device</t>
   </si>
@@ -744,6 +746,176 @@
   </si>
   <si>
     <t>Red</t>
+  </si>
+  <si>
+    <t>Relay Break</t>
+  </si>
+  <si>
+    <t>E-14</t>
+  </si>
+  <si>
+    <t>C-3</t>
+  </si>
+  <si>
+    <t>Break when Advance Unit is at 0</t>
+  </si>
+  <si>
+    <t>W-3</t>
+  </si>
+  <si>
+    <t>R-BLU-2</t>
+  </si>
+  <si>
+    <t>BLU-O-1</t>
+  </si>
+  <si>
+    <t>Advance Unit Reset</t>
+  </si>
+  <si>
+    <t>Outhole Relay</t>
+  </si>
+  <si>
+    <t>Reset Relay</t>
+  </si>
+  <si>
+    <t>Rocket Special</t>
+  </si>
+  <si>
+    <t>Change</t>
+  </si>
+  <si>
+    <t>100000 Pt</t>
+  </si>
+  <si>
+    <t>1000 Pt</t>
+  </si>
+  <si>
+    <t>100 Pt</t>
+  </si>
+  <si>
+    <t>10 Pt</t>
+  </si>
+  <si>
+    <t>5-Balls-in-Line</t>
+  </si>
+  <si>
+    <t>Double Bonus</t>
+  </si>
+  <si>
+    <t>Y-BR-3</t>
+  </si>
+  <si>
+    <t>R-BR</t>
+  </si>
+  <si>
+    <t>B-W</t>
+  </si>
+  <si>
+    <t>R-W-4</t>
+  </si>
+  <si>
+    <t>G-B-1</t>
+  </si>
+  <si>
+    <t>GREY-O-1</t>
+  </si>
+  <si>
+    <t>Spacelab Special Adj</t>
+  </si>
+  <si>
+    <t>Spacelab Relay</t>
+  </si>
+  <si>
+    <t>Score Motor 6-B</t>
+  </si>
+  <si>
+    <t>B-G-3</t>
+  </si>
+  <si>
+    <t>R-G-4</t>
+  </si>
+  <si>
+    <t>GREY-R</t>
+  </si>
+  <si>
+    <t>GREY-2</t>
+  </si>
+  <si>
+    <t>BR-G-2</t>
+  </si>
+  <si>
+    <t>Rocket Special Adj</t>
+  </si>
+  <si>
+    <t>5-Balls-In-Line</t>
+  </si>
+  <si>
+    <t>GREY-BL-4</t>
+  </si>
+  <si>
+    <t>Captive Ball Latch/Trip</t>
+  </si>
+  <si>
+    <t>A-M</t>
+  </si>
+  <si>
+    <t>B-M</t>
+  </si>
+  <si>
+    <t>A-B</t>
+  </si>
+  <si>
+    <t>B-B</t>
+  </si>
+  <si>
+    <t>F-M</t>
+  </si>
+  <si>
+    <t>F-B</t>
+  </si>
+  <si>
+    <t>W-1</t>
+  </si>
+  <si>
+    <t>1,000 Point</t>
+  </si>
+  <si>
+    <t>Spacelab Spec. / 1,000 Point</t>
+  </si>
+  <si>
+    <t>1,000 Point Relay</t>
+  </si>
+  <si>
+    <t>Advance Stepup</t>
+  </si>
+  <si>
+    <t>B-D-2</t>
+  </si>
+  <si>
+    <t>GREY-B-3</t>
+  </si>
+  <si>
+    <t>BLU-Y-3</t>
+  </si>
+  <si>
+    <t>R Top Rollover Light
+L Bot Rollover Light</t>
+  </si>
+  <si>
+    <t>L Top Rollover Light
+R Bot Rollover Light</t>
+  </si>
+  <si>
+    <t>L Bot SpecvLight</t>
+  </si>
+  <si>
+    <t>R Bot SpecvLight</t>
+  </si>
+  <si>
+    <t>Captive Ball</t>
+  </si>
+  <si>
+    <t>Break when Score Motor 5-G</t>
   </si>
 </sst>
 </file>
@@ -792,12 +964,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
@@ -1113,10 +1286,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90CD940A-D4A1-4744-A54A-1B3E70AA0E2C}">
-  <dimension ref="A1:H105"/>
+  <dimension ref="A1:I156"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
-      <selection activeCell="H95" sqref="H95"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1127,24 +1300,25 @@
     <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9.33203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="20.109375" customWidth="1"/>
+    <col min="9" max="9" width="16.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>0</v>
       </c>
@@ -1169,8 +1343,11 @@
       <c r="H5" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I5" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -1187,7 +1364,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -1213,7 +1390,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>3</v>
       </c>
@@ -1236,7 +1413,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>3</v>
       </c>
@@ -1259,7 +1436,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>3</v>
       </c>
@@ -1282,7 +1459,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>3</v>
       </c>
@@ -1305,7 +1482,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>33</v>
       </c>
@@ -1322,7 +1499,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>33</v>
       </c>
@@ -1348,7 +1525,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>33</v>
       </c>
@@ -1374,7 +1551,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>33</v>
       </c>
@@ -1400,7 +1577,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>33</v>
       </c>
@@ -1824,7 +2001,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>97</v>
       </c>
@@ -1841,7 +2018,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>97</v>
       </c>
@@ -1867,7 +2044,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>97</v>
       </c>
@@ -1893,7 +2070,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>97</v>
       </c>
@@ -1919,7 +2096,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>97</v>
       </c>
@@ -1945,7 +2122,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>97</v>
       </c>
@@ -1971,7 +2148,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>105</v>
       </c>
@@ -1988,7 +2165,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>105</v>
       </c>
@@ -2013,8 +2190,11 @@
       <c r="H40" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I40" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>105</v>
       </c>
@@ -2040,7 +2220,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>105</v>
       </c>
@@ -2066,7 +2246,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>105</v>
       </c>
@@ -2092,7 +2272,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>117</v>
       </c>
@@ -2103,7 +2283,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>117</v>
       </c>
@@ -2128,8 +2308,11 @@
       <c r="H45" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I45" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>117</v>
       </c>
@@ -2155,7 +2338,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>117</v>
       </c>
@@ -2181,7 +2364,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>124</v>
       </c>
@@ -3191,13 +3374,16 @@
         <v>129</v>
       </c>
     </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A97" s="1" t="s">
         <v>211</v>
       </c>
       <c r="B97" t="s">
         <v>2</v>
       </c>
+      <c r="E97" t="s">
+        <v>218</v>
+      </c>
       <c r="F97" t="s">
         <v>219</v>
       </c>
@@ -3205,7 +3391,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A98" s="1" t="s">
         <v>211</v>
       </c>
@@ -3231,7 +3417,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A99" s="1" t="s">
         <v>211</v>
       </c>
@@ -3257,7 +3443,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A100" s="1" t="s">
         <v>211</v>
       </c>
@@ -3283,7 +3469,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A101" s="1" t="s">
         <v>211</v>
       </c>
@@ -3309,7 +3495,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A102" s="1" t="s">
         <v>211</v>
       </c>
@@ -3335,7 +3521,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A103" s="1" t="s">
         <v>211</v>
       </c>
@@ -3361,7 +3547,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A104" s="1" t="s">
         <v>211</v>
       </c>
@@ -3387,7 +3573,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A105" s="1" t="s">
         <v>211</v>
       </c>
@@ -3411,6 +3597,1029 @@
       </c>
       <c r="H105" t="s">
         <v>230</v>
+      </c>
+    </row>
+    <row r="106" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A106" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B106" t="s">
+        <v>2</v>
+      </c>
+      <c r="D106" t="s">
+        <v>38</v>
+      </c>
+      <c r="F106" t="s">
+        <v>43</v>
+      </c>
+      <c r="G106" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="107" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A107" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B107" t="s">
+        <v>155</v>
+      </c>
+      <c r="C107" t="s">
+        <v>15</v>
+      </c>
+      <c r="D107" t="s">
+        <v>38</v>
+      </c>
+      <c r="E107" t="s">
+        <v>25</v>
+      </c>
+      <c r="F107" t="s">
+        <v>42</v>
+      </c>
+      <c r="G107" t="s">
+        <v>43</v>
+      </c>
+      <c r="H107" t="s">
+        <v>59</v>
+      </c>
+      <c r="I107" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="108" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A108" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B108" t="s">
+        <v>155</v>
+      </c>
+      <c r="C108" t="s">
+        <v>17</v>
+      </c>
+      <c r="D108" t="s">
+        <v>150</v>
+      </c>
+      <c r="E108" t="s">
+        <v>25</v>
+      </c>
+      <c r="F108" t="s">
+        <v>239</v>
+      </c>
+      <c r="G108" t="s">
+        <v>240</v>
+      </c>
+      <c r="H108" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="109" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A109" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B109" t="s">
+        <v>155</v>
+      </c>
+      <c r="C109" t="s">
+        <v>18</v>
+      </c>
+      <c r="D109" t="s">
+        <v>235</v>
+      </c>
+      <c r="E109" t="s">
+        <v>25</v>
+      </c>
+      <c r="F109" t="s">
+        <v>121</v>
+      </c>
+      <c r="G109" t="s">
+        <v>223</v>
+      </c>
+      <c r="H109" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="110" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A110" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B110" t="s">
+        <v>155</v>
+      </c>
+      <c r="C110" t="s">
+        <v>19</v>
+      </c>
+      <c r="D110" t="s">
+        <v>39</v>
+      </c>
+      <c r="E110" t="s">
+        <v>25</v>
+      </c>
+      <c r="F110" t="s">
+        <v>58</v>
+      </c>
+      <c r="G110" t="s">
+        <v>46</v>
+      </c>
+      <c r="H110" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="111" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A111" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B111" t="s">
+        <v>155</v>
+      </c>
+      <c r="C111" t="s">
+        <v>20</v>
+      </c>
+      <c r="D111" t="s">
+        <v>236</v>
+      </c>
+      <c r="E111" t="s">
+        <v>25</v>
+      </c>
+      <c r="F111" t="s">
+        <v>58</v>
+      </c>
+      <c r="G111" t="s">
+        <v>35</v>
+      </c>
+      <c r="H111" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="112" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A112" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B112" t="s">
+        <v>155</v>
+      </c>
+      <c r="C112" t="s">
+        <v>50</v>
+      </c>
+      <c r="D112" t="s">
+        <v>38</v>
+      </c>
+      <c r="E112" t="s">
+        <v>26</v>
+      </c>
+      <c r="F112" t="s">
+        <v>238</v>
+      </c>
+      <c r="G112" t="s">
+        <v>75</v>
+      </c>
+      <c r="H112" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="113" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A113" t="s">
+        <v>226</v>
+      </c>
+      <c r="B113" t="s">
+        <v>2</v>
+      </c>
+      <c r="D113" t="s">
+        <v>215</v>
+      </c>
+      <c r="F113" t="s">
+        <v>221</v>
+      </c>
+      <c r="G113" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="114" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A114" t="s">
+        <v>226</v>
+      </c>
+      <c r="B114" t="s">
+        <v>155</v>
+      </c>
+      <c r="C114" t="s">
+        <v>15</v>
+      </c>
+      <c r="D114" t="s">
+        <v>180</v>
+      </c>
+      <c r="E114" t="s">
+        <v>25</v>
+      </c>
+      <c r="F114" t="s">
+        <v>253</v>
+      </c>
+      <c r="G114" t="s">
+        <v>221</v>
+      </c>
+      <c r="H114" t="s">
+        <v>59</v>
+      </c>
+      <c r="I114" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="115" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A115" t="s">
+        <v>226</v>
+      </c>
+      <c r="B115" t="s">
+        <v>155</v>
+      </c>
+      <c r="C115" t="s">
+        <v>17</v>
+      </c>
+      <c r="D115" t="s">
+        <v>12</v>
+      </c>
+      <c r="E115" t="s">
+        <v>25</v>
+      </c>
+      <c r="F115" t="s">
+        <v>254</v>
+      </c>
+      <c r="G115" t="s">
+        <v>255</v>
+      </c>
+      <c r="H115" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="116" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A116" t="s">
+        <v>226</v>
+      </c>
+      <c r="B116" t="s">
+        <v>155</v>
+      </c>
+      <c r="C116" t="s">
+        <v>18</v>
+      </c>
+      <c r="D116" t="s">
+        <v>37</v>
+      </c>
+      <c r="E116" t="s">
+        <v>25</v>
+      </c>
+      <c r="F116" t="s">
+        <v>256</v>
+      </c>
+      <c r="G116" t="s">
+        <v>257</v>
+      </c>
+      <c r="H116" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="117" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A117" t="s">
+        <v>226</v>
+      </c>
+      <c r="B117" t="s">
+        <v>155</v>
+      </c>
+      <c r="C117" t="s">
+        <v>19</v>
+      </c>
+      <c r="D117" t="s">
+        <v>39</v>
+      </c>
+      <c r="E117" t="s">
+        <v>25</v>
+      </c>
+      <c r="F117" t="s">
+        <v>58</v>
+      </c>
+      <c r="G117" t="s">
+        <v>159</v>
+      </c>
+      <c r="H117" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="118" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A118" t="s">
+        <v>226</v>
+      </c>
+      <c r="B118" t="s">
+        <v>155</v>
+      </c>
+      <c r="C118" t="s">
+        <v>20</v>
+      </c>
+      <c r="D118" t="s">
+        <v>180</v>
+      </c>
+      <c r="E118" t="s">
+        <v>26</v>
+      </c>
+      <c r="F118" t="s">
+        <v>58</v>
+      </c>
+      <c r="G118" t="s">
+        <v>252</v>
+      </c>
+      <c r="H118" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="119" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A119" t="s">
+        <v>244</v>
+      </c>
+      <c r="B119" t="s">
+        <v>2</v>
+      </c>
+      <c r="D119" t="s">
+        <v>108</v>
+      </c>
+      <c r="F119" t="s">
+        <v>261</v>
+      </c>
+      <c r="G119" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="120" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A120" t="s">
+        <v>244</v>
+      </c>
+      <c r="B120" t="s">
+        <v>155</v>
+      </c>
+      <c r="C120" t="s">
+        <v>15</v>
+      </c>
+      <c r="D120" t="s">
+        <v>118</v>
+      </c>
+      <c r="E120" t="s">
+        <v>25</v>
+      </c>
+      <c r="F120" t="s">
+        <v>109</v>
+      </c>
+      <c r="G120" t="s">
+        <v>261</v>
+      </c>
+      <c r="H120" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="121" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A121" t="s">
+        <v>244</v>
+      </c>
+      <c r="B121" t="s">
+        <v>155</v>
+      </c>
+      <c r="C121" t="s">
+        <v>17</v>
+      </c>
+      <c r="D121" t="s">
+        <v>12</v>
+      </c>
+      <c r="E121" t="s">
+        <v>25</v>
+      </c>
+      <c r="F121" t="s">
+        <v>254</v>
+      </c>
+      <c r="G121" t="s">
+        <v>262</v>
+      </c>
+      <c r="H121" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="122" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A122" t="s">
+        <v>244</v>
+      </c>
+      <c r="B122" t="s">
+        <v>155</v>
+      </c>
+      <c r="C122" t="s">
+        <v>18</v>
+      </c>
+      <c r="D122" t="s">
+        <v>37</v>
+      </c>
+      <c r="E122" t="s">
+        <v>25</v>
+      </c>
+      <c r="F122" t="s">
+        <v>263</v>
+      </c>
+      <c r="G122" t="s">
+        <v>265</v>
+      </c>
+      <c r="H122" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="123" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A123" t="s">
+        <v>244</v>
+      </c>
+      <c r="B123" t="s">
+        <v>155</v>
+      </c>
+      <c r="C123" t="s">
+        <v>19</v>
+      </c>
+      <c r="D123" t="s">
+        <v>39</v>
+      </c>
+      <c r="E123" t="s">
+        <v>25</v>
+      </c>
+      <c r="F123" t="s">
+        <v>58</v>
+      </c>
+      <c r="G123" t="s">
+        <v>46</v>
+      </c>
+      <c r="H123" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="124" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A124" t="s">
+        <v>244</v>
+      </c>
+      <c r="B124" t="s">
+        <v>155</v>
+      </c>
+      <c r="C124" t="s">
+        <v>20</v>
+      </c>
+      <c r="D124" t="s">
+        <v>98</v>
+      </c>
+      <c r="E124" t="s">
+        <v>25</v>
+      </c>
+      <c r="F124" t="s">
+        <v>87</v>
+      </c>
+      <c r="G124" t="s">
+        <v>257</v>
+      </c>
+      <c r="H124" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="125" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A125" t="s">
+        <v>244</v>
+      </c>
+      <c r="B125" t="s">
+        <v>155</v>
+      </c>
+      <c r="C125" t="s">
+        <v>50</v>
+      </c>
+      <c r="D125" t="s">
+        <v>52</v>
+      </c>
+      <c r="E125" t="s">
+        <v>25</v>
+      </c>
+      <c r="F125" t="s">
+        <v>268</v>
+      </c>
+      <c r="G125" t="s">
+        <v>64</v>
+      </c>
+      <c r="H125" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="126" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A126" t="s">
+        <v>245</v>
+      </c>
+      <c r="B126" t="s">
+        <v>2</v>
+      </c>
+      <c r="F126" t="s">
+        <v>276</v>
+      </c>
+      <c r="G126" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="127" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A127" t="s">
+        <v>245</v>
+      </c>
+      <c r="B127" t="s">
+        <v>155</v>
+      </c>
+      <c r="C127" t="s">
+        <v>270</v>
+      </c>
+      <c r="D127" t="s">
+        <v>119</v>
+      </c>
+      <c r="E127" t="s">
+        <v>25</v>
+      </c>
+      <c r="F127" t="s">
+        <v>183</v>
+      </c>
+      <c r="G127" t="s">
+        <v>223</v>
+      </c>
+      <c r="H127" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="128" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A128" t="s">
+        <v>245</v>
+      </c>
+      <c r="B128" t="s">
+        <v>155</v>
+      </c>
+      <c r="C128" t="s">
+        <v>272</v>
+      </c>
+      <c r="D128" t="s">
+        <v>119</v>
+      </c>
+      <c r="E128" t="s">
+        <v>26</v>
+      </c>
+      <c r="F128" t="s">
+        <v>183</v>
+      </c>
+      <c r="G128" t="s">
+        <v>222</v>
+      </c>
+      <c r="H128" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="129" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A129" t="s">
+        <v>245</v>
+      </c>
+      <c r="B129" t="s">
+        <v>155</v>
+      </c>
+      <c r="C129" t="s">
+        <v>271</v>
+      </c>
+      <c r="D129" t="s">
+        <v>119</v>
+      </c>
+      <c r="E129" t="s">
+        <v>25</v>
+      </c>
+      <c r="F129" t="s">
+        <v>184</v>
+      </c>
+      <c r="G129" t="s">
+        <v>222</v>
+      </c>
+      <c r="H129" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="130" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A130" t="s">
+        <v>245</v>
+      </c>
+      <c r="B130" t="s">
+        <v>155</v>
+      </c>
+      <c r="C130" t="s">
+        <v>273</v>
+      </c>
+      <c r="D130" t="s">
+        <v>119</v>
+      </c>
+      <c r="E130" t="s">
+        <v>26</v>
+      </c>
+      <c r="F130" t="s">
+        <v>184</v>
+      </c>
+      <c r="G130" t="s">
+        <v>223</v>
+      </c>
+      <c r="H130" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="131" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A131" t="s">
+        <v>245</v>
+      </c>
+      <c r="B131" t="s">
+        <v>155</v>
+      </c>
+      <c r="C131" t="s">
+        <v>212</v>
+      </c>
+      <c r="D131" t="s">
+        <v>107</v>
+      </c>
+      <c r="E131" t="s">
+        <v>25</v>
+      </c>
+      <c r="F131" t="s">
+        <v>200</v>
+      </c>
+      <c r="G131" t="s">
+        <v>196</v>
+      </c>
+      <c r="H131" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="132" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A132" t="s">
+        <v>245</v>
+      </c>
+      <c r="B132" t="s">
+        <v>155</v>
+      </c>
+      <c r="C132" t="s">
+        <v>213</v>
+      </c>
+      <c r="D132" t="s">
+        <v>107</v>
+      </c>
+      <c r="E132" t="s">
+        <v>26</v>
+      </c>
+      <c r="F132" t="s">
+        <v>200</v>
+      </c>
+      <c r="G132" t="s">
+        <v>115</v>
+      </c>
+      <c r="H132" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="133" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A133" t="s">
+        <v>245</v>
+      </c>
+      <c r="B133" t="s">
+        <v>155</v>
+      </c>
+      <c r="C133" t="s">
+        <v>78</v>
+      </c>
+      <c r="D133" t="s">
+        <v>107</v>
+      </c>
+      <c r="E133" t="s">
+        <v>25</v>
+      </c>
+      <c r="F133" t="s">
+        <v>201</v>
+      </c>
+      <c r="G133" t="s">
+        <v>115</v>
+      </c>
+      <c r="H133" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="134" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A134" t="s">
+        <v>245</v>
+      </c>
+      <c r="B134" t="s">
+        <v>155</v>
+      </c>
+      <c r="C134" t="s">
+        <v>79</v>
+      </c>
+      <c r="D134" t="s">
+        <v>107</v>
+      </c>
+      <c r="E134" t="s">
+        <v>26</v>
+      </c>
+      <c r="F134" t="s">
+        <v>201</v>
+      </c>
+      <c r="G134" t="s">
+        <v>196</v>
+      </c>
+      <c r="H134" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="135" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A135" t="s">
+        <v>245</v>
+      </c>
+      <c r="B135" t="s">
+        <v>155</v>
+      </c>
+      <c r="C135" t="s">
+        <v>80</v>
+      </c>
+      <c r="D135" t="s">
+        <v>214</v>
+      </c>
+      <c r="E135" t="s">
+        <v>25</v>
+      </c>
+      <c r="F135" t="s">
+        <v>58</v>
+      </c>
+      <c r="G135" t="s">
+        <v>264</v>
+      </c>
+      <c r="H135" s="1" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="136" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A136" t="s">
+        <v>245</v>
+      </c>
+      <c r="B136" t="s">
+        <v>155</v>
+      </c>
+      <c r="C136" t="s">
+        <v>81</v>
+      </c>
+      <c r="D136" t="s">
+        <v>214</v>
+      </c>
+      <c r="E136" t="s">
+        <v>26</v>
+      </c>
+      <c r="F136" t="s">
+        <v>58</v>
+      </c>
+      <c r="G136" t="s">
+        <v>281</v>
+      </c>
+      <c r="H136" s="1" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="137" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A137" t="s">
+        <v>245</v>
+      </c>
+      <c r="B137" t="s">
+        <v>155</v>
+      </c>
+      <c r="C137" t="s">
+        <v>274</v>
+      </c>
+      <c r="D137" t="s">
+        <v>214</v>
+      </c>
+      <c r="E137" t="s">
+        <v>25</v>
+      </c>
+      <c r="F137" t="s">
+        <v>220</v>
+      </c>
+      <c r="G137" t="s">
+        <v>282</v>
+      </c>
+      <c r="H137" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="138" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A138" t="s">
+        <v>245</v>
+      </c>
+      <c r="B138" t="s">
+        <v>155</v>
+      </c>
+      <c r="C138" t="s">
+        <v>275</v>
+      </c>
+      <c r="D138" t="s">
+        <v>214</v>
+      </c>
+      <c r="E138" t="s">
+        <v>26</v>
+      </c>
+      <c r="F138" t="s">
+        <v>220</v>
+      </c>
+      <c r="G138" t="s">
+        <v>283</v>
+      </c>
+      <c r="H138" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="139" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A139" t="s">
+        <v>288</v>
+      </c>
+      <c r="B139" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="140" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A140" t="s">
+        <v>288</v>
+      </c>
+      <c r="B140" t="s">
+        <v>155</v>
+      </c>
+      <c r="C140" t="s">
+        <v>270</v>
+      </c>
+      <c r="D140" t="s">
+        <v>217</v>
+      </c>
+      <c r="E140" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="141" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A141" t="s">
+        <v>288</v>
+      </c>
+      <c r="B141" t="s">
+        <v>155</v>
+      </c>
+      <c r="C141" t="s">
+        <v>272</v>
+      </c>
+      <c r="D141" t="s">
+        <v>217</v>
+      </c>
+      <c r="E141" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="142" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A142" t="s">
+        <v>288</v>
+      </c>
+      <c r="B142" t="s">
+        <v>155</v>
+      </c>
+      <c r="C142" t="s">
+        <v>271</v>
+      </c>
+      <c r="D142" t="s">
+        <v>191</v>
+      </c>
+      <c r="E142" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="143" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A143" t="s">
+        <v>288</v>
+      </c>
+      <c r="B143" t="s">
+        <v>155</v>
+      </c>
+      <c r="C143" t="s">
+        <v>273</v>
+      </c>
+      <c r="D143" t="s">
+        <v>191</v>
+      </c>
+      <c r="E143" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="144" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A144" t="s">
+        <v>288</v>
+      </c>
+      <c r="B144" t="s">
+        <v>155</v>
+      </c>
+      <c r="C144" t="s">
+        <v>212</v>
+      </c>
+      <c r="D144" t="s">
+        <v>106</v>
+      </c>
+      <c r="E144" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="145" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A145" t="s">
+        <v>288</v>
+      </c>
+      <c r="B145" t="s">
+        <v>155</v>
+      </c>
+      <c r="C145" t="s">
+        <v>213</v>
+      </c>
+      <c r="D145" t="s">
+        <v>106</v>
+      </c>
+      <c r="E145" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="146" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A146" t="s">
+        <v>60</v>
+      </c>
+      <c r="B146" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="147" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A147" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="B147" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="148" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A148" t="s">
+        <v>247</v>
+      </c>
+      <c r="B148" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="149" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A149" t="s">
+        <v>248</v>
+      </c>
+      <c r="B149" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="150" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A150" t="s">
+        <v>249</v>
+      </c>
+      <c r="B150" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="151" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A151" t="s">
+        <v>250</v>
+      </c>
+      <c r="B151" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="152" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A152" t="s">
+        <v>154</v>
+      </c>
+      <c r="B152" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="153" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A153" t="s">
+        <v>162</v>
+      </c>
+      <c r="B153" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="154" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A154" t="s">
+        <v>251</v>
+      </c>
+      <c r="B154" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="155" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A155" t="s">
+        <v>44</v>
+      </c>
+      <c r="B155" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="156" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A156" t="s">
+        <v>211</v>
+      </c>
+      <c r="B156" t="s">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>